<commit_message>
Site updated: 2020-07-21 09:09:29
</commit_message>
<xml_diff>
--- a/data/totaltime (1).xlsx
+++ b/data/totaltime (1).xlsx
@@ -393,13 +393,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>127</v>
+        <v>230</v>
       </c>
       <c r="B2" t="str">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="C2" t="str">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>